<commit_message>
aggiunto light schema a foscarini
</commit_message>
<xml_diff>
--- a/xls/flos/result/flos_aumentato.xlsx
+++ b/xls/flos/result/flos_aumentato.xlsx
@@ -10186,6 +10186,9 @@
       <x:c r="W2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X2" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y2" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
@@ -10248,6 +10251,9 @@
       <x:c r="W3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X3" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y3" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
@@ -10310,6 +10316,9 @@
       <x:c r="W4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X4" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y4" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
@@ -10372,6 +10381,9 @@
       <x:c r="W5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X5" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y5" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
@@ -10434,6 +10446,9 @@
       <x:c r="W6" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X6" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y6" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
@@ -10496,6 +10511,9 @@
       <x:c r="W7" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X7" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y7" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
@@ -10558,6 +10576,9 @@
       <x:c r="W8" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X8" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y8" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
@@ -10620,6 +10641,9 @@
       <x:c r="W9" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X9" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y9" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
@@ -10682,6 +10706,9 @@
       <x:c r="W10" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X10" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y10" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
@@ -10744,6 +10771,9 @@
       <x:c r="W11" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X11" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y11" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
@@ -10806,6 +10836,9 @@
       <x:c r="W12" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X12" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y12" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
@@ -10868,6 +10901,9 @@
       <x:c r="W13" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X13" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y13" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
@@ -10930,6 +10966,9 @@
       <x:c r="W14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X14" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y14" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
@@ -10992,6 +11031,9 @@
       <x:c r="W15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X15" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y15" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
@@ -11054,6 +11096,9 @@
       <x:c r="W16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X16" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y16" s="0" t="s">
         <x:v>129</x:v>
       </x:c>
@@ -11116,6 +11161,9 @@
       <x:c r="W17" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X17" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y17" s="0" t="s">
         <x:v>139</x:v>
       </x:c>
@@ -11178,6 +11226,9 @@
       <x:c r="W18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X18" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y18" s="0" t="s">
         <x:v>148</x:v>
       </x:c>
@@ -11240,6 +11291,9 @@
       <x:c r="W19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X19" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y19" s="0" t="s">
         <x:v>157</x:v>
       </x:c>
@@ -11302,6 +11356,9 @@
       <x:c r="W20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X20" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y20" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
@@ -11364,6 +11421,9 @@
       <x:c r="W21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X21" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y21" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
@@ -11426,6 +11486,9 @@
       <x:c r="W22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X22" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y22" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
@@ -11488,6 +11551,9 @@
       <x:c r="W23" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X23" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y23" s="0" t="s">
         <x:v>187</x:v>
       </x:c>
@@ -11550,6 +11616,9 @@
       <x:c r="W24" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X24" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y24" s="0" t="s">
         <x:v>187</x:v>
       </x:c>
@@ -11612,6 +11681,9 @@
       <x:c r="W25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X25" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y25" s="0" t="s">
         <x:v>187</x:v>
       </x:c>
@@ -11671,6 +11743,9 @@
       <x:c r="W26" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X26" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y26" s="0" t="s">
         <x:v>206</x:v>
       </x:c>
@@ -11724,6 +11799,9 @@
       <x:c r="W27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X27" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y27" s="0" t="s">
         <x:v>213</x:v>
       </x:c>
@@ -11777,6 +11855,9 @@
       <x:c r="W28" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X28" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y28" s="0" t="s">
         <x:v>219</x:v>
       </x:c>
@@ -11833,6 +11914,9 @@
       <x:c r="W29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X29" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y29" s="0" t="s">
         <x:v>225</x:v>
       </x:c>
@@ -11895,6 +11979,9 @@
       <x:c r="W30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X30" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y30" s="0" t="s">
         <x:v>225</x:v>
       </x:c>
@@ -11957,6 +12044,9 @@
       <x:c r="W31" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X31" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y31" s="0" t="s">
         <x:v>225</x:v>
       </x:c>
@@ -12019,6 +12109,9 @@
       <x:c r="W32" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X32" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y32" s="0" t="s">
         <x:v>245</x:v>
       </x:c>
@@ -12081,6 +12174,9 @@
       <x:c r="W33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X33" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y33" s="0" t="s">
         <x:v>245</x:v>
       </x:c>
@@ -12143,6 +12239,9 @@
       <x:c r="W34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X34" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y34" s="0" t="s">
         <x:v>245</x:v>
       </x:c>
@@ -12205,6 +12304,9 @@
       <x:c r="W35" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X35" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y35" s="0" t="s">
         <x:v>263</x:v>
       </x:c>
@@ -12267,6 +12369,9 @@
       <x:c r="W36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X36" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y36" s="0" t="s">
         <x:v>263</x:v>
       </x:c>
@@ -12329,6 +12434,9 @@
       <x:c r="W37" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X37" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y37" s="0" t="s">
         <x:v>263</x:v>
       </x:c>
@@ -12391,6 +12499,9 @@
       <x:c r="W38" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X38" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y38" s="0" t="s">
         <x:v>283</x:v>
       </x:c>
@@ -12453,6 +12564,9 @@
       <x:c r="W39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X39" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y39" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
@@ -12515,6 +12629,9 @@
       <x:c r="W40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X40" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y40" s="0" t="s">
         <x:v>302</x:v>
       </x:c>
@@ -12577,6 +12694,9 @@
       <x:c r="W41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X41" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y41" s="0" t="s">
         <x:v>310</x:v>
       </x:c>
@@ -12639,6 +12759,9 @@
       <x:c r="W42" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X42" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y42" s="0" t="s">
         <x:v>320</x:v>
       </x:c>
@@ -12701,6 +12824,9 @@
       <x:c r="W43" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X43" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y43" s="0" t="s">
         <x:v>329</x:v>
       </x:c>
@@ -12763,6 +12889,9 @@
       <x:c r="W44" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X44" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y44" s="0" t="s">
         <x:v>336</x:v>
       </x:c>
@@ -12825,6 +12954,9 @@
       <x:c r="W45" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X45" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y45" s="0" t="s">
         <x:v>344</x:v>
       </x:c>
@@ -12887,6 +13019,9 @@
       <x:c r="W46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X46" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y46" s="0" t="s">
         <x:v>352</x:v>
       </x:c>
@@ -12949,6 +13084,9 @@
       <x:c r="W47" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X47" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y47" s="0" t="s">
         <x:v>360</x:v>
       </x:c>
@@ -13011,6 +13149,9 @@
       <x:c r="W48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X48" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y48" s="0" t="s">
         <x:v>367</x:v>
       </x:c>
@@ -13073,6 +13214,9 @@
       <x:c r="W49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X49" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y49" s="0" t="s">
         <x:v>375</x:v>
       </x:c>
@@ -13135,6 +13279,9 @@
       <x:c r="W50" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X50" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y50" s="0" t="s">
         <x:v>382</x:v>
       </x:c>
@@ -13191,6 +13338,9 @@
       <x:c r="W51" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X51" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y51" s="0" t="s">
         <x:v>389</x:v>
       </x:c>
@@ -13241,6 +13391,9 @@
       <x:c r="W52" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X52" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y52" s="0" t="s">
         <x:v>394</x:v>
       </x:c>
@@ -13291,6 +13444,9 @@
       <x:c r="W53" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X53" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y53" s="0" t="s">
         <x:v>400</x:v>
       </x:c>
@@ -13347,6 +13503,9 @@
       <x:c r="W54" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X54" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y54" s="0" t="s">
         <x:v>406</x:v>
       </x:c>
@@ -13409,6 +13568,9 @@
       <x:c r="W55" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X55" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y55" s="0" t="s">
         <x:v>413</x:v>
       </x:c>
@@ -13471,6 +13633,9 @@
       <x:c r="W56" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X56" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y56" s="0" t="s">
         <x:v>421</x:v>
       </x:c>
@@ -13533,6 +13698,9 @@
       <x:c r="W57" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X57" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y57" s="0" t="s">
         <x:v>431</x:v>
       </x:c>
@@ -13595,6 +13763,9 @@
       <x:c r="W58" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X58" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y58" s="0" t="s">
         <x:v>431</x:v>
       </x:c>
@@ -13657,6 +13828,9 @@
       <x:c r="W59" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X59" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y59" s="0" t="s">
         <x:v>431</x:v>
       </x:c>
@@ -13719,6 +13893,9 @@
       <x:c r="W60" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X60" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y60" s="0" t="s">
         <x:v>431</x:v>
       </x:c>
@@ -13781,6 +13958,9 @@
       <x:c r="W61" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X61" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y61" s="0" t="s">
         <x:v>431</x:v>
       </x:c>
@@ -13843,6 +14023,9 @@
       <x:c r="W62" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X62" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y62" s="0" t="s">
         <x:v>465</x:v>
       </x:c>
@@ -13905,6 +14088,9 @@
       <x:c r="W63" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X63" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y63" s="0" t="s">
         <x:v>465</x:v>
       </x:c>
@@ -13967,6 +14153,9 @@
       <x:c r="W64" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X64" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y64" s="0" t="s">
         <x:v>465</x:v>
       </x:c>
@@ -14029,6 +14218,9 @@
       <x:c r="W65" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X65" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y65" s="0" t="s">
         <x:v>465</x:v>
       </x:c>
@@ -14088,6 +14280,9 @@
       <x:c r="W66" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X66" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y66" s="0" t="s">
         <x:v>493</x:v>
       </x:c>
@@ -14141,6 +14336,9 @@
       <x:c r="W67" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X67" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y67" s="0" t="s">
         <x:v>500</x:v>
       </x:c>
@@ -14194,6 +14392,9 @@
       <x:c r="W68" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X68" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y68" s="0" t="s">
         <x:v>507</x:v>
       </x:c>
@@ -14247,6 +14448,9 @@
       <x:c r="W69" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X69" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y69" s="0" t="s">
         <x:v>513</x:v>
       </x:c>
@@ -14300,6 +14504,9 @@
       <x:c r="W70" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X70" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y70" s="0" t="s">
         <x:v>520</x:v>
       </x:c>
@@ -14353,6 +14560,9 @@
       <x:c r="W71" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X71" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y71" s="0" t="s">
         <x:v>526</x:v>
       </x:c>
@@ -14406,6 +14616,9 @@
       <x:c r="W72" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X72" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y72" s="0" t="s">
         <x:v>493</x:v>
       </x:c>
@@ -14459,6 +14672,9 @@
       <x:c r="W73" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X73" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y73" s="0" t="s">
         <x:v>500</x:v>
       </x:c>
@@ -14512,6 +14728,9 @@
       <x:c r="W74" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X74" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y74" s="0" t="s">
         <x:v>507</x:v>
       </x:c>
@@ -14565,6 +14784,9 @@
       <x:c r="W75" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X75" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y75" s="0" t="s">
         <x:v>513</x:v>
       </x:c>
@@ -14615,6 +14837,9 @@
       <x:c r="W76" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X76" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y76" s="0" t="s">
         <x:v>552</x:v>
       </x:c>
@@ -14668,6 +14893,9 @@
       <x:c r="W77" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X77" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y77" s="0" t="s">
         <x:v>520</x:v>
       </x:c>
@@ -14721,6 +14949,9 @@
       <x:c r="W78" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X78" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y78" s="0" t="s">
         <x:v>526</x:v>
       </x:c>
@@ -14777,6 +15008,9 @@
       <x:c r="W79" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X79" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y79" s="0" t="s">
         <x:v>565</x:v>
       </x:c>
@@ -14839,6 +15073,9 @@
       <x:c r="W80" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X80" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y80" s="0" t="s">
         <x:v>565</x:v>
       </x:c>
@@ -14901,6 +15138,9 @@
       <x:c r="W81" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X81" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y81" s="0" t="s">
         <x:v>565</x:v>
       </x:c>
@@ -14963,6 +15203,9 @@
       <x:c r="W82" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X82" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y82" s="0" t="s">
         <x:v>565</x:v>
       </x:c>
@@ -15025,6 +15268,9 @@
       <x:c r="W83" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X83" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y83" s="0" t="s">
         <x:v>587</x:v>
       </x:c>
@@ -15087,6 +15333,9 @@
       <x:c r="W84" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X84" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y84" s="0" t="s">
         <x:v>587</x:v>
       </x:c>
@@ -15149,6 +15398,9 @@
       <x:c r="W85" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X85" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y85" s="0" t="s">
         <x:v>602</x:v>
       </x:c>
@@ -15211,6 +15463,9 @@
       <x:c r="W86" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X86" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y86" s="0" t="s">
         <x:v>602</x:v>
       </x:c>
@@ -15273,6 +15528,9 @@
       <x:c r="W87" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X87" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y87" s="0" t="s">
         <x:v>616</x:v>
       </x:c>
@@ -15335,6 +15593,9 @@
       <x:c r="W88" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X88" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y88" s="0" t="s">
         <x:v>616</x:v>
       </x:c>
@@ -15397,6 +15658,9 @@
       <x:c r="W89" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X89" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y89" s="0" t="s">
         <x:v>616</x:v>
       </x:c>
@@ -15459,6 +15723,9 @@
       <x:c r="W90" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X90" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y90" s="0" t="s">
         <x:v>616</x:v>
       </x:c>
@@ -15521,6 +15788,9 @@
       <x:c r="W91" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X91" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y91" s="0" t="s">
         <x:v>643</x:v>
       </x:c>
@@ -15583,6 +15853,9 @@
       <x:c r="W92" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X92" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y92" s="0" t="s">
         <x:v>643</x:v>
       </x:c>
@@ -15645,6 +15918,9 @@
       <x:c r="W93" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X93" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y93" s="0" t="s">
         <x:v>643</x:v>
       </x:c>
@@ -15707,6 +15983,9 @@
       <x:c r="W94" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X94" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y94" s="0" t="s">
         <x:v>663</x:v>
       </x:c>
@@ -15769,6 +16048,9 @@
       <x:c r="W95" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X95" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y95" s="0" t="s">
         <x:v>663</x:v>
       </x:c>
@@ -15831,6 +16113,9 @@
       <x:c r="W96" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X96" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y96" s="0" t="s">
         <x:v>663</x:v>
       </x:c>
@@ -15893,6 +16178,9 @@
       <x:c r="W97" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X97" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y97" s="0" t="s">
         <x:v>682</x:v>
       </x:c>
@@ -15955,6 +16243,9 @@
       <x:c r="W98" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X98" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y98" s="0" t="s">
         <x:v>682</x:v>
       </x:c>
@@ -16017,6 +16308,9 @@
       <x:c r="W99" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X99" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y99" s="0" t="s">
         <x:v>682</x:v>
       </x:c>
@@ -16079,6 +16373,9 @@
       <x:c r="W100" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X100" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y100" s="0" t="s">
         <x:v>700</x:v>
       </x:c>
@@ -16141,6 +16438,9 @@
       <x:c r="W101" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X101" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y101" s="0" t="s">
         <x:v>700</x:v>
       </x:c>
@@ -16203,6 +16503,9 @@
       <x:c r="W102" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X102" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y102" s="0" t="s">
         <x:v>700</x:v>
       </x:c>
@@ -16265,6 +16568,9 @@
       <x:c r="W103" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X103" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y103" s="0" t="s">
         <x:v>717</x:v>
       </x:c>
@@ -16327,6 +16633,9 @@
       <x:c r="W104" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X104" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y104" s="0" t="s">
         <x:v>717</x:v>
       </x:c>
@@ -16389,6 +16698,9 @@
       <x:c r="W105" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X105" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y105" s="0" t="s">
         <x:v>717</x:v>
       </x:c>
@@ -16451,6 +16763,9 @@
       <x:c r="W106" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X106" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y106" s="0" t="s">
         <x:v>732</x:v>
       </x:c>
@@ -16513,6 +16828,9 @@
       <x:c r="W107" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X107" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y107" s="0" t="s">
         <x:v>732</x:v>
       </x:c>
@@ -16575,6 +16893,9 @@
       <x:c r="W108" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X108" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y108" s="0" t="s">
         <x:v>732</x:v>
       </x:c>
@@ -16637,6 +16958,9 @@
       <x:c r="W109" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X109" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y109" s="0" t="s">
         <x:v>747</x:v>
       </x:c>
@@ -16699,6 +17023,9 @@
       <x:c r="W110" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X110" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y110" s="0" t="s">
         <x:v>747</x:v>
       </x:c>
@@ -16761,6 +17088,9 @@
       <x:c r="W111" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X111" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y111" s="0" t="s">
         <x:v>763</x:v>
       </x:c>
@@ -16823,6 +17153,9 @@
       <x:c r="W112" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X112" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y112" s="0" t="s">
         <x:v>763</x:v>
       </x:c>
@@ -16885,6 +17218,9 @@
       <x:c r="W113" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X113" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y113" s="0" t="s">
         <x:v>779</x:v>
       </x:c>
@@ -16944,6 +17280,9 @@
       <x:c r="W114" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X114" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y114" s="0" t="s">
         <x:v>788</x:v>
       </x:c>
@@ -16997,6 +17336,9 @@
       <x:c r="W115" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X115" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y115" s="0" t="s">
         <x:v>794</x:v>
       </x:c>
@@ -17050,6 +17392,9 @@
       <x:c r="W116" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X116" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y116" s="0" t="s">
         <x:v>801</x:v>
       </x:c>
@@ -17103,6 +17448,9 @@
       <x:c r="W117" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X117" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y117" s="0" t="s">
         <x:v>807</x:v>
       </x:c>
@@ -17159,6 +17507,9 @@
       <x:c r="W118" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X118" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y118" s="0" t="s">
         <x:v>814</x:v>
       </x:c>
@@ -17221,6 +17572,9 @@
       <x:c r="W119" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X119" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y119" s="0" t="s">
         <x:v>814</x:v>
       </x:c>
@@ -17283,6 +17637,9 @@
       <x:c r="W120" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X120" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y120" s="0" t="s">
         <x:v>814</x:v>
       </x:c>
@@ -17345,6 +17702,9 @@
       <x:c r="W121" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X121" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y121" s="0" t="s">
         <x:v>814</x:v>
       </x:c>
@@ -17407,6 +17767,9 @@
       <x:c r="W122" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X122" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y122" s="0" t="s">
         <x:v>838</x:v>
       </x:c>
@@ -17469,6 +17832,9 @@
       <x:c r="W123" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X123" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y123" s="0" t="s">
         <x:v>838</x:v>
       </x:c>
@@ -17531,6 +17897,9 @@
       <x:c r="W124" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X124" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y124" s="0" t="s">
         <x:v>838</x:v>
       </x:c>
@@ -17593,6 +17962,9 @@
       <x:c r="W125" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X125" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y125" s="0" t="s">
         <x:v>838</x:v>
       </x:c>
@@ -17655,6 +18027,9 @@
       <x:c r="W126" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X126" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y126" s="0" t="s">
         <x:v>860</x:v>
       </x:c>
@@ -17717,6 +18092,9 @@
       <x:c r="W127" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X127" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y127" s="0" t="s">
         <x:v>860</x:v>
       </x:c>
@@ -17779,6 +18157,9 @@
       <x:c r="W128" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X128" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y128" s="0" t="s">
         <x:v>874</x:v>
       </x:c>
@@ -17841,6 +18222,9 @@
       <x:c r="W129" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X129" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y129" s="0" t="s">
         <x:v>884</x:v>
       </x:c>
@@ -17903,6 +18287,9 @@
       <x:c r="W130" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X130" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y130" s="0" t="s">
         <x:v>893</x:v>
       </x:c>
@@ -17965,6 +18352,9 @@
       <x:c r="W131" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X131" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y131" s="0" t="s">
         <x:v>893</x:v>
       </x:c>
@@ -18027,6 +18417,9 @@
       <x:c r="W132" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X132" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y132" s="0" t="s">
         <x:v>893</x:v>
       </x:c>
@@ -18089,6 +18482,9 @@
       <x:c r="W133" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X133" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y133" s="0" t="s">
         <x:v>893</x:v>
       </x:c>
@@ -18151,6 +18547,9 @@
       <x:c r="W134" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X134" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y134" s="0" t="s">
         <x:v>919</x:v>
       </x:c>
@@ -18213,6 +18612,9 @@
       <x:c r="W135" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X135" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y135" s="0" t="s">
         <x:v>928</x:v>
       </x:c>
@@ -18275,6 +18677,9 @@
       <x:c r="W136" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X136" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y136" s="0" t="s">
         <x:v>928</x:v>
       </x:c>
@@ -18337,6 +18742,9 @@
       <x:c r="W137" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X137" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y137" s="0" t="s">
         <x:v>928</x:v>
       </x:c>
@@ -18399,6 +18807,9 @@
       <x:c r="W138" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X138" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y138" s="0" t="s">
         <x:v>950</x:v>
       </x:c>
@@ -18461,6 +18872,9 @@
       <x:c r="W139" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X139" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y139" s="0" t="s">
         <x:v>958</x:v>
       </x:c>
@@ -18523,6 +18937,9 @@
       <x:c r="W140" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X140" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y140" s="0" t="s">
         <x:v>958</x:v>
       </x:c>
@@ -18585,6 +19002,9 @@
       <x:c r="W141" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X141" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y141" s="0" t="s">
         <x:v>958</x:v>
       </x:c>
@@ -18647,6 +19067,9 @@
       <x:c r="W142" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X142" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y142" s="0" t="s">
         <x:v>979</x:v>
       </x:c>
@@ -18709,6 +19132,9 @@
       <x:c r="W143" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X143" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y143" s="0" t="s">
         <x:v>988</x:v>
       </x:c>
@@ -18771,6 +19197,9 @@
       <x:c r="W144" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X144" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y144" s="0" t="s">
         <x:v>996</x:v>
       </x:c>
@@ -18833,6 +19262,9 @@
       <x:c r="W145" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X145" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y145" s="0" t="s">
         <x:v>1005</x:v>
       </x:c>
@@ -18895,6 +19327,9 @@
       <x:c r="W146" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X146" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y146" s="0" t="s">
         <x:v>1013</x:v>
       </x:c>
@@ -18957,6 +19392,9 @@
       <x:c r="W147" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X147" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y147" s="0" t="s">
         <x:v>1022</x:v>
       </x:c>
@@ -19019,6 +19457,9 @@
       <x:c r="W148" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X148" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y148" s="0" t="s">
         <x:v>1022</x:v>
       </x:c>
@@ -19081,6 +19522,9 @@
       <x:c r="W149" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X149" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y149" s="0" t="s">
         <x:v>1036</x:v>
       </x:c>
@@ -19143,6 +19587,9 @@
       <x:c r="W150" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X150" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y150" s="0" t="s">
         <x:v>1036</x:v>
       </x:c>
@@ -19199,6 +19646,9 @@
       <x:c r="W151" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X151" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y151" s="0" t="s">
         <x:v>1050</x:v>
       </x:c>
@@ -19249,6 +19699,9 @@
       <x:c r="W152" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X152" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y152" s="0" t="s">
         <x:v>1056</x:v>
       </x:c>
@@ -19299,6 +19752,9 @@
       <x:c r="W153" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X153" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y153" s="0" t="s">
         <x:v>1061</x:v>
       </x:c>
@@ -19349,6 +19805,9 @@
       <x:c r="W154" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X154" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y154" s="0" t="s">
         <x:v>1066</x:v>
       </x:c>
@@ -19399,6 +19858,9 @@
       <x:c r="W155" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X155" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y155" s="0" t="s">
         <x:v>1071</x:v>
       </x:c>
@@ -19449,6 +19911,9 @@
       <x:c r="W156" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X156" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y156" s="0" t="s">
         <x:v>1076</x:v>
       </x:c>
@@ -19499,6 +19964,9 @@
       <x:c r="W157" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X157" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y157" s="0" t="s">
         <x:v>1081</x:v>
       </x:c>
@@ -19549,6 +20017,9 @@
       <x:c r="W158" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X158" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y158" s="0" t="s">
         <x:v>1086</x:v>
       </x:c>
@@ -19599,6 +20070,9 @@
       <x:c r="W159" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X159" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y159" s="0" t="s">
         <x:v>1091</x:v>
       </x:c>
@@ -19649,6 +20123,9 @@
       <x:c r="W160" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X160" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y160" s="0" t="s">
         <x:v>1097</x:v>
       </x:c>
@@ -19705,6 +20182,9 @@
       <x:c r="W161" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X161" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y161" s="0" t="s">
         <x:v>1102</x:v>
       </x:c>
@@ -19767,6 +20247,9 @@
       <x:c r="W162" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X162" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y162" s="0" t="s">
         <x:v>1110</x:v>
       </x:c>
@@ -19829,6 +20312,9 @@
       <x:c r="W163" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X163" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y163" s="0" t="s">
         <x:v>1117</x:v>
       </x:c>
@@ -19891,6 +20377,9 @@
       <x:c r="W164" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X164" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y164" s="0" t="s">
         <x:v>1117</x:v>
       </x:c>
@@ -19953,6 +20442,9 @@
       <x:c r="W165" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X165" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y165" s="0" t="s">
         <x:v>1132</x:v>
       </x:c>
@@ -20015,6 +20507,9 @@
       <x:c r="W166" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X166" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y166" s="0" t="s">
         <x:v>1132</x:v>
       </x:c>
@@ -20077,6 +20572,9 @@
       <x:c r="W167" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X167" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y167" s="0" t="s">
         <x:v>1145</x:v>
       </x:c>
@@ -20139,6 +20637,9 @@
       <x:c r="W168" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X168" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y168" s="0" t="s">
         <x:v>1145</x:v>
       </x:c>
@@ -20201,6 +20702,9 @@
       <x:c r="W169" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X169" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y169" s="0" t="s">
         <x:v>1159</x:v>
       </x:c>
@@ -20263,6 +20767,9 @@
       <x:c r="W170" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X170" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y170" s="0" t="s">
         <x:v>1167</x:v>
       </x:c>
@@ -20325,6 +20832,9 @@
       <x:c r="W171" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X171" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y171" s="0" t="s">
         <x:v>1175</x:v>
       </x:c>
@@ -20387,6 +20897,9 @@
       <x:c r="W172" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X172" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y172" s="0" t="s">
         <x:v>1182</x:v>
       </x:c>
@@ -20449,6 +20962,9 @@
       <x:c r="W173" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X173" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y173" s="0" t="s">
         <x:v>1192</x:v>
       </x:c>
@@ -20511,6 +21027,9 @@
       <x:c r="W174" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X174" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y174" s="0" t="s">
         <x:v>1200</x:v>
       </x:c>
@@ -20573,6 +21092,9 @@
       <x:c r="W175" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X175" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y175" s="0" t="s">
         <x:v>1208</x:v>
       </x:c>
@@ -20635,6 +21157,9 @@
       <x:c r="W176" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X176" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y176" s="0" t="s">
         <x:v>1216</x:v>
       </x:c>
@@ -20697,6 +21222,9 @@
       <x:c r="W177" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X177" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y177" s="0" t="s">
         <x:v>1224</x:v>
       </x:c>
@@ -20759,6 +21287,9 @@
       <x:c r="W178" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X178" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y178" s="0" t="s">
         <x:v>1231</x:v>
       </x:c>
@@ -20821,6 +21352,9 @@
       <x:c r="W179" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X179" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y179" s="0" t="s">
         <x:v>1239</x:v>
       </x:c>
@@ -20883,6 +21417,9 @@
       <x:c r="W180" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X180" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y180" s="0" t="s">
         <x:v>1248</x:v>
       </x:c>
@@ -20945,6 +21482,9 @@
       <x:c r="W181" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X181" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y181" s="0" t="s">
         <x:v>1256</x:v>
       </x:c>
@@ -21001,6 +21541,9 @@
       <x:c r="W182" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X182" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y182" s="0" t="s">
         <x:v>1263</x:v>
       </x:c>
@@ -21057,6 +21600,9 @@
       <x:c r="W183" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="X183" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y183" s="0" t="s">
         <x:v>1270</x:v>
       </x:c>
@@ -21119,6 +21665,9 @@
       <x:c r="W184" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="X184" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y184" s="0" t="s">
         <x:v>1270</x:v>
       </x:c>
@@ -21181,6 +21730,9 @@
       <x:c r="W185" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="X185" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y185" s="0" t="s">
         <x:v>1270</x:v>
       </x:c>
@@ -21243,6 +21795,9 @@
       <x:c r="W186" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X186" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y186" s="0" t="s">
         <x:v>1290</x:v>
       </x:c>
@@ -21305,6 +21860,9 @@
       <x:c r="W187" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X187" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y187" s="0" t="s">
         <x:v>1290</x:v>
       </x:c>
@@ -21367,6 +21925,9 @@
       <x:c r="W188" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X188" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y188" s="0" t="s">
         <x:v>1290</x:v>
       </x:c>
@@ -21429,6 +21990,9 @@
       <x:c r="W189" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X189" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y189" s="0" t="s">
         <x:v>1310</x:v>
       </x:c>
@@ -21491,6 +22055,9 @@
       <x:c r="W190" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X190" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y190" s="0" t="s">
         <x:v>1310</x:v>
       </x:c>
@@ -21553,6 +22120,9 @@
       <x:c r="W191" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X191" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y191" s="0" t="s">
         <x:v>1310</x:v>
       </x:c>
@@ -21615,6 +22185,9 @@
       <x:c r="W192" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X192" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y192" s="0" t="s">
         <x:v>1327</x:v>
       </x:c>
@@ -21677,6 +22250,9 @@
       <x:c r="W193" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X193" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y193" s="0" t="s">
         <x:v>1327</x:v>
       </x:c>
@@ -21739,6 +22315,9 @@
       <x:c r="W194" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X194" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y194" s="0" t="s">
         <x:v>1327</x:v>
       </x:c>
@@ -21801,6 +22380,9 @@
       <x:c r="W195" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X195" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y195" s="0" t="s">
         <x:v>1344</x:v>
       </x:c>
@@ -21863,6 +22445,9 @@
       <x:c r="W196" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X196" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y196" s="0" t="s">
         <x:v>1344</x:v>
       </x:c>
@@ -21925,6 +22510,9 @@
       <x:c r="W197" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X197" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y197" s="0" t="s">
         <x:v>1344</x:v>
       </x:c>
@@ -21987,6 +22575,9 @@
       <x:c r="W198" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X198" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y198" s="0" t="s">
         <x:v>1362</x:v>
       </x:c>
@@ -22049,6 +22640,9 @@
       <x:c r="W199" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X199" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y199" s="0" t="s">
         <x:v>1362</x:v>
       </x:c>
@@ -22111,6 +22705,9 @@
       <x:c r="W200" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X200" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y200" s="0" t="s">
         <x:v>1362</x:v>
       </x:c>
@@ -22173,6 +22770,9 @@
       <x:c r="W201" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X201" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y201" s="0" t="s">
         <x:v>1379</x:v>
       </x:c>
@@ -22235,6 +22835,9 @@
       <x:c r="W202" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X202" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y202" s="0" t="s">
         <x:v>1379</x:v>
       </x:c>
@@ -22297,6 +22900,9 @@
       <x:c r="W203" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X203" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y203" s="0" t="s">
         <x:v>1379</x:v>
       </x:c>
@@ -22359,6 +22965,9 @@
       <x:c r="W204" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X204" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y204" s="0" t="s">
         <x:v>1397</x:v>
       </x:c>
@@ -22421,6 +23030,9 @@
       <x:c r="W205" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X205" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y205" s="0" t="s">
         <x:v>1397</x:v>
       </x:c>
@@ -22483,6 +23095,9 @@
       <x:c r="W206" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X206" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y206" s="0" t="s">
         <x:v>1397</x:v>
       </x:c>
@@ -22545,6 +23160,9 @@
       <x:c r="W207" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X207" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y207" s="0" t="s">
         <x:v>1414</x:v>
       </x:c>
@@ -22607,6 +23225,9 @@
       <x:c r="W208" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X208" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y208" s="0" t="s">
         <x:v>1414</x:v>
       </x:c>
@@ -22669,6 +23290,9 @@
       <x:c r="W209" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X209" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y209" s="0" t="s">
         <x:v>1414</x:v>
       </x:c>
@@ -22731,6 +23355,9 @@
       <x:c r="W210" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X210" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y210" s="0" t="s">
         <x:v>1433</x:v>
       </x:c>
@@ -22793,6 +23420,9 @@
       <x:c r="W211" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X211" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y211" s="0" t="s">
         <x:v>1433</x:v>
       </x:c>
@@ -22855,6 +23485,9 @@
       <x:c r="W212" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X212" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y212" s="0" t="s">
         <x:v>1433</x:v>
       </x:c>
@@ -22917,6 +23550,9 @@
       <x:c r="W213" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X213" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y213" s="0" t="s">
         <x:v>1450</x:v>
       </x:c>
@@ -22979,6 +23615,9 @@
       <x:c r="W214" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X214" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y214" s="0" t="s">
         <x:v>1459</x:v>
       </x:c>
@@ -23041,6 +23680,9 @@
       <x:c r="W215" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X215" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y215" s="0" t="s">
         <x:v>1467</x:v>
       </x:c>
@@ -23103,6 +23745,9 @@
       <x:c r="W216" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X216" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y216" s="0" t="s">
         <x:v>1467</x:v>
       </x:c>
@@ -23165,6 +23810,9 @@
       <x:c r="W217" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X217" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y217" s="0" t="s">
         <x:v>1482</x:v>
       </x:c>
@@ -23227,6 +23875,9 @@
       <x:c r="W218" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X218" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y218" s="0" t="s">
         <x:v>1482</x:v>
       </x:c>
@@ -23289,6 +23940,9 @@
       <x:c r="W219" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X219" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y219" s="0" t="s">
         <x:v>1482</x:v>
       </x:c>
@@ -23351,6 +24005,9 @@
       <x:c r="W220" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X220" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y220" s="0" t="s">
         <x:v>1503</x:v>
       </x:c>
@@ -23413,6 +24070,9 @@
       <x:c r="W221" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X221" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y221" s="0" t="s">
         <x:v>1503</x:v>
       </x:c>
@@ -23475,6 +24135,9 @@
       <x:c r="W222" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X222" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y222" s="0" t="s">
         <x:v>1503</x:v>
       </x:c>
@@ -23537,6 +24200,9 @@
       <x:c r="W223" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X223" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y223" s="0" t="s">
         <x:v>1521</x:v>
       </x:c>
@@ -23599,6 +24265,9 @@
       <x:c r="W224" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X224" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y224" s="0" t="s">
         <x:v>1521</x:v>
       </x:c>
@@ -23661,6 +24330,9 @@
       <x:c r="W225" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X225" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y225" s="0" t="s">
         <x:v>1521</x:v>
       </x:c>
@@ -23723,6 +24395,9 @@
       <x:c r="W226" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X226" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y226" s="0" t="s">
         <x:v>1540</x:v>
       </x:c>
@@ -23785,6 +24460,9 @@
       <x:c r="W227" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X227" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y227" s="0" t="s">
         <x:v>1540</x:v>
       </x:c>
@@ -23847,6 +24525,9 @@
       <x:c r="W228" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X228" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y228" s="0" t="s">
         <x:v>1540</x:v>
       </x:c>
@@ -23909,6 +24590,9 @@
       <x:c r="W229" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X229" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y229" s="0" t="s">
         <x:v>1540</x:v>
       </x:c>
@@ -23971,6 +24655,9 @@
       <x:c r="W230" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X230" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y230" s="0" t="s">
         <x:v>1563</x:v>
       </x:c>
@@ -24033,6 +24720,9 @@
       <x:c r="W231" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X231" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y231" s="0" t="s">
         <x:v>1563</x:v>
       </x:c>
@@ -24095,6 +24785,9 @@
       <x:c r="W232" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X232" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y232" s="0" t="s">
         <x:v>1563</x:v>
       </x:c>
@@ -24157,6 +24850,9 @@
       <x:c r="W233" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X233" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y233" s="0" t="s">
         <x:v>1563</x:v>
       </x:c>
@@ -24219,6 +24915,9 @@
       <x:c r="W234" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X234" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y234" s="0" t="s">
         <x:v>1585</x:v>
       </x:c>
@@ -24281,6 +24980,9 @@
       <x:c r="W235" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X235" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y235" s="0" t="s">
         <x:v>1585</x:v>
       </x:c>
@@ -24343,6 +25045,9 @@
       <x:c r="W236" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X236" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y236" s="0" t="s">
         <x:v>1585</x:v>
       </x:c>
@@ -24405,6 +25110,9 @@
       <x:c r="W237" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X237" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y237" s="0" t="s">
         <x:v>1585</x:v>
       </x:c>
@@ -24467,6 +25175,9 @@
       <x:c r="W238" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X238" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y238" s="0" t="s">
         <x:v>1482</x:v>
       </x:c>
@@ -24529,6 +25240,9 @@
       <x:c r="W239" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X239" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y239" s="0" t="s">
         <x:v>1503</x:v>
       </x:c>
@@ -24591,6 +25305,9 @@
       <x:c r="W240" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X240" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y240" s="0" t="s">
         <x:v>1618</x:v>
       </x:c>
@@ -24653,6 +25370,9 @@
       <x:c r="W241" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X241" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y241" s="0" t="s">
         <x:v>1626</x:v>
       </x:c>
@@ -24715,6 +25435,9 @@
       <x:c r="W242" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X242" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y242" s="0" t="s">
         <x:v>1634</x:v>
       </x:c>
@@ -24777,6 +25500,9 @@
       <x:c r="W243" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X243" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y243" s="0" t="s">
         <x:v>1642</x:v>
       </x:c>
@@ -24839,6 +25565,9 @@
       <x:c r="W244" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X244" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y244" s="0" t="s">
         <x:v>1650</x:v>
       </x:c>
@@ -24901,6 +25630,9 @@
       <x:c r="W245" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X245" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y245" s="0" t="s">
         <x:v>1659</x:v>
       </x:c>
@@ -24963,6 +25695,9 @@
       <x:c r="W246" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X246" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y246" s="0" t="s">
         <x:v>1659</x:v>
       </x:c>
@@ -25025,6 +25760,9 @@
       <x:c r="W247" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X247" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y247" s="0" t="s">
         <x:v>1674</x:v>
       </x:c>
@@ -25087,6 +25825,9 @@
       <x:c r="W248" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X248" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y248" s="0" t="s">
         <x:v>1674</x:v>
       </x:c>
@@ -25149,6 +25890,9 @@
       <x:c r="W249" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X249" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y249" s="0" t="s">
         <x:v>1674</x:v>
       </x:c>
@@ -25211,6 +25955,9 @@
       <x:c r="W250" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X250" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y250" s="0" t="s">
         <x:v>1674</x:v>
       </x:c>
@@ -25273,6 +26020,9 @@
       <x:c r="W251" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X251" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y251" s="0" t="s">
         <x:v>1699</x:v>
       </x:c>
@@ -25335,6 +26085,9 @@
       <x:c r="W252" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X252" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y252" s="0" t="s">
         <x:v>1699</x:v>
       </x:c>
@@ -25397,6 +26150,9 @@
       <x:c r="W253" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X253" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y253" s="0" t="s">
         <x:v>1699</x:v>
       </x:c>
@@ -25459,6 +26215,9 @@
       <x:c r="W254" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X254" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y254" s="0" t="s">
         <x:v>1699</x:v>
       </x:c>
@@ -25521,6 +26280,9 @@
       <x:c r="W255" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X255" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y255" s="0" t="s">
         <x:v>1721</x:v>
       </x:c>
@@ -25583,6 +26345,9 @@
       <x:c r="W256" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X256" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y256" s="0" t="s">
         <x:v>1721</x:v>
       </x:c>
@@ -25645,6 +26410,9 @@
       <x:c r="W257" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X257" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y257" s="0" t="s">
         <x:v>1721</x:v>
       </x:c>
@@ -25707,6 +26475,9 @@
       <x:c r="W258" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X258" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y258" s="0" t="s">
         <x:v>1721</x:v>
       </x:c>
@@ -25769,6 +26540,9 @@
       <x:c r="W259" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X259" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y259" s="0" t="s">
         <x:v>1743</x:v>
       </x:c>
@@ -25831,6 +26605,9 @@
       <x:c r="W260" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X260" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y260" s="0" t="s">
         <x:v>1743</x:v>
       </x:c>
@@ -25893,6 +26670,9 @@
       <x:c r="W261" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X261" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y261" s="0" t="s">
         <x:v>1743</x:v>
       </x:c>
@@ -25955,6 +26735,9 @@
       <x:c r="W262" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X262" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y262" s="0" t="s">
         <x:v>1743</x:v>
       </x:c>
@@ -26017,6 +26800,9 @@
       <x:c r="W263" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X263" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y263" s="0" t="s">
         <x:v>1765</x:v>
       </x:c>
@@ -26079,6 +26865,9 @@
       <x:c r="W264" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X264" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y264" s="0" t="s">
         <x:v>1765</x:v>
       </x:c>
@@ -26141,6 +26930,9 @@
       <x:c r="W265" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X265" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y265" s="0" t="s">
         <x:v>1765</x:v>
       </x:c>
@@ -26203,6 +26995,9 @@
       <x:c r="W266" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X266" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y266" s="0" t="s">
         <x:v>1765</x:v>
       </x:c>
@@ -26265,6 +27060,9 @@
       <x:c r="W267" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X267" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y267" s="0" t="s">
         <x:v>1787</x:v>
       </x:c>
@@ -26327,6 +27125,9 @@
       <x:c r="W268" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X268" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y268" s="0" t="s">
         <x:v>1795</x:v>
       </x:c>
@@ -26389,6 +27190,9 @@
       <x:c r="W269" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X269" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y269" s="0" t="s">
         <x:v>1795</x:v>
       </x:c>
@@ -26451,6 +27255,9 @@
       <x:c r="W270" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X270" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y270" s="0" t="s">
         <x:v>1808</x:v>
       </x:c>
@@ -26513,6 +27320,9 @@
       <x:c r="W271" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X271" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y271" s="0" t="s">
         <x:v>1816</x:v>
       </x:c>
@@ -26575,6 +27385,9 @@
       <x:c r="W272" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X272" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y272" s="0" t="s">
         <x:v>1823</x:v>
       </x:c>
@@ -26637,6 +27450,9 @@
       <x:c r="W273" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X273" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y273" s="0" t="s">
         <x:v>1831</x:v>
       </x:c>
@@ -26699,6 +27515,9 @@
       <x:c r="W274" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X274" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y274" s="0" t="s">
         <x:v>1839</x:v>
       </x:c>
@@ -26761,6 +27580,9 @@
       <x:c r="W275" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X275" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y275" s="0" t="s">
         <x:v>1848</x:v>
       </x:c>
@@ -26823,6 +27645,9 @@
       <x:c r="W276" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X276" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y276" s="0" t="s">
         <x:v>1856</x:v>
       </x:c>
@@ -26885,6 +27710,9 @@
       <x:c r="W277" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X277" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y277" s="0" t="s">
         <x:v>1865</x:v>
       </x:c>
@@ -26947,6 +27775,9 @@
       <x:c r="W278" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X278" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y278" s="0" t="s">
         <x:v>1874</x:v>
       </x:c>
@@ -27009,6 +27840,9 @@
       <x:c r="W279" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X279" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y279" s="0" t="s">
         <x:v>1883</x:v>
       </x:c>
@@ -27071,6 +27905,9 @@
       <x:c r="W280" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X280" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y280" s="0" t="s">
         <x:v>1891</x:v>
       </x:c>
@@ -27133,6 +27970,9 @@
       <x:c r="W281" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X281" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y281" s="0" t="s">
         <x:v>1891</x:v>
       </x:c>
@@ -27195,6 +28035,9 @@
       <x:c r="W282" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X282" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y282" s="0" t="s">
         <x:v>1891</x:v>
       </x:c>
@@ -27257,6 +28100,9 @@
       <x:c r="W283" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X283" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y283" s="0" t="s">
         <x:v>1891</x:v>
       </x:c>
@@ -27319,6 +28165,9 @@
       <x:c r="W284" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X284" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y284" s="0" t="s">
         <x:v>1916</x:v>
       </x:c>
@@ -27381,6 +28230,9 @@
       <x:c r="W285" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X285" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y285" s="0" t="s">
         <x:v>1924</x:v>
       </x:c>
@@ -27443,6 +28295,9 @@
       <x:c r="W286" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X286" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y286" s="0" t="s">
         <x:v>1924</x:v>
       </x:c>
@@ -27505,6 +28360,9 @@
       <x:c r="W287" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X287" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y287" s="0" t="s">
         <x:v>1924</x:v>
       </x:c>
@@ -27567,6 +28425,9 @@
       <x:c r="W288" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X288" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y288" s="0" t="s">
         <x:v>1924</x:v>
       </x:c>
@@ -27626,6 +28487,9 @@
       <x:c r="W289" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X289" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y289" s="0" t="s">
         <x:v>1950</x:v>
       </x:c>
@@ -27679,6 +28543,9 @@
       <x:c r="W290" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X290" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y290" s="0" t="s">
         <x:v>1955</x:v>
       </x:c>
@@ -27732,6 +28599,9 @@
       <x:c r="W291" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X291" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y291" s="0" t="s">
         <x:v>1960</x:v>
       </x:c>
@@ -27785,6 +28655,9 @@
       <x:c r="W292" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X292" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y292" s="0" t="s">
         <x:v>1966</x:v>
       </x:c>
@@ -27841,6 +28714,9 @@
       <x:c r="W293" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X293" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y293" s="0" t="s">
         <x:v>1972</x:v>
       </x:c>
@@ -27903,6 +28779,9 @@
       <x:c r="W294" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X294" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y294" s="0" t="s">
         <x:v>1972</x:v>
       </x:c>
@@ -27965,6 +28844,9 @@
       <x:c r="W295" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X295" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y295" s="0" t="s">
         <x:v>1972</x:v>
       </x:c>
@@ -28027,6 +28909,9 @@
       <x:c r="W296" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X296" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y296" s="0" t="s">
         <x:v>1972</x:v>
       </x:c>
@@ -28086,6 +28971,9 @@
       <x:c r="W297" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X297" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y297" s="0" t="s">
         <x:v>1995</x:v>
       </x:c>
@@ -28139,6 +29027,9 @@
       <x:c r="W298" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X298" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y298" s="0" t="s">
         <x:v>2000</x:v>
       </x:c>
@@ -28192,6 +29083,9 @@
       <x:c r="W299" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X299" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y299" s="0" t="s">
         <x:v>2005</x:v>
       </x:c>
@@ -28245,6 +29139,9 @@
       <x:c r="W300" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X300" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y300" s="0" t="s">
         <x:v>2010</x:v>
       </x:c>
@@ -28301,6 +29198,9 @@
       <x:c r="W301" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X301" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y301" s="0" t="s">
         <x:v>2016</x:v>
       </x:c>
@@ -28363,6 +29263,9 @@
       <x:c r="W302" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X302" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y302" s="0" t="s">
         <x:v>2016</x:v>
       </x:c>
@@ -28425,6 +29328,9 @@
       <x:c r="W303" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X303" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y303" s="0" t="s">
         <x:v>2016</x:v>
       </x:c>
@@ -28487,6 +29393,9 @@
       <x:c r="W304" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X304" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y304" s="0" t="s">
         <x:v>2016</x:v>
       </x:c>
@@ -28549,6 +29458,9 @@
       <x:c r="W305" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X305" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y305" s="0" t="s">
         <x:v>2040</x:v>
       </x:c>
@@ -28611,6 +29523,9 @@
       <x:c r="W306" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X306" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y306" s="0" t="s">
         <x:v>2040</x:v>
       </x:c>
@@ -28673,6 +29588,9 @@
       <x:c r="W307" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X307" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y307" s="0" t="s">
         <x:v>2057</x:v>
       </x:c>
@@ -28735,6 +29653,9 @@
       <x:c r="W308" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X308" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y308" s="0" t="s">
         <x:v>2057</x:v>
       </x:c>
@@ -28797,6 +29718,9 @@
       <x:c r="W309" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X309" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y309" s="0" t="s">
         <x:v>2057</x:v>
       </x:c>
@@ -28859,6 +29783,9 @@
       <x:c r="W310" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X310" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y310" s="0" t="s">
         <x:v>2076</x:v>
       </x:c>
@@ -28921,6 +29848,9 @@
       <x:c r="W311" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X311" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y311" s="0" t="s">
         <x:v>2076</x:v>
       </x:c>
@@ -28983,6 +29913,9 @@
       <x:c r="W312" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X312" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y312" s="0" t="s">
         <x:v>2076</x:v>
       </x:c>
@@ -29045,6 +29978,9 @@
       <x:c r="W313" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X313" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y313" s="0" t="s">
         <x:v>2095</x:v>
       </x:c>
@@ -29107,6 +30043,9 @@
       <x:c r="W314" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X314" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y314" s="0" t="s">
         <x:v>2095</x:v>
       </x:c>
@@ -29169,6 +30108,9 @@
       <x:c r="W315" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X315" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y315" s="0" t="s">
         <x:v>2095</x:v>
       </x:c>
@@ -29231,6 +30173,9 @@
       <x:c r="W316" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X316" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y316" s="0" t="s">
         <x:v>2115</x:v>
       </x:c>
@@ -29293,6 +30238,9 @@
       <x:c r="W317" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X317" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y317" s="0" t="s">
         <x:v>2115</x:v>
       </x:c>
@@ -29355,6 +30303,9 @@
       <x:c r="W318" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X318" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y318" s="0" t="s">
         <x:v>2115</x:v>
       </x:c>
@@ -29417,6 +30368,9 @@
       <x:c r="W319" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X319" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y319" s="0" t="s">
         <x:v>2134</x:v>
       </x:c>
@@ -29479,6 +30433,9 @@
       <x:c r="W320" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X320" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y320" s="0" t="s">
         <x:v>2141</x:v>
       </x:c>
@@ -29541,6 +30498,9 @@
       <x:c r="W321" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X321" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y321" s="0" t="s">
         <x:v>2149</x:v>
       </x:c>
@@ -29603,6 +30563,9 @@
       <x:c r="W322" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X322" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y322" s="0" t="s">
         <x:v>2157</x:v>
       </x:c>
@@ -29665,6 +30628,9 @@
       <x:c r="W323" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X323" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y323" s="0" t="s">
         <x:v>2165</x:v>
       </x:c>
@@ -29727,6 +30693,9 @@
       <x:c r="W324" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X324" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y324" s="0" t="s">
         <x:v>2173</x:v>
       </x:c>
@@ -29789,6 +30758,9 @@
       <x:c r="W325" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X325" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y325" s="0" t="s">
         <x:v>2181</x:v>
       </x:c>
@@ -29851,6 +30823,9 @@
       <x:c r="W326" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X326" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y326" s="0" t="s">
         <x:v>2188</x:v>
       </x:c>
@@ -29913,6 +30888,9 @@
       <x:c r="W327" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X327" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y327" s="0" t="s">
         <x:v>2196</x:v>
       </x:c>
@@ -29975,6 +30953,9 @@
       <x:c r="W328" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X328" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y328" s="0" t="s">
         <x:v>2204</x:v>
       </x:c>
@@ -30037,6 +31018,9 @@
       <x:c r="W329" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X329" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y329" s="0" t="s">
         <x:v>2212</x:v>
       </x:c>
@@ -30099,6 +31083,9 @@
       <x:c r="W330" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X330" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y330" s="0" t="s">
         <x:v>2212</x:v>
       </x:c>
@@ -30161,6 +31148,9 @@
       <x:c r="W331" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X331" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y331" s="0" t="s">
         <x:v>2227</x:v>
       </x:c>
@@ -30223,6 +31213,9 @@
       <x:c r="W332" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X332" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y332" s="0" t="s">
         <x:v>2227</x:v>
       </x:c>
@@ -30285,6 +31278,9 @@
       <x:c r="W333" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X333" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y333" s="0" t="s">
         <x:v>2227</x:v>
       </x:c>
@@ -30347,6 +31343,9 @@
       <x:c r="W334" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X334" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y334" s="0" t="s">
         <x:v>2227</x:v>
       </x:c>
@@ -30409,6 +31408,9 @@
       <x:c r="W335" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X335" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y335" s="0" t="s">
         <x:v>2252</x:v>
       </x:c>
@@ -30471,6 +31473,9 @@
       <x:c r="W336" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X336" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y336" s="0" t="s">
         <x:v>2252</x:v>
       </x:c>
@@ -30533,6 +31538,9 @@
       <x:c r="W337" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X337" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y337" s="0" t="s">
         <x:v>2265</x:v>
       </x:c>
@@ -30595,6 +31603,9 @@
       <x:c r="W338" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X338" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y338" s="0" t="s">
         <x:v>2265</x:v>
       </x:c>
@@ -30657,6 +31668,9 @@
       <x:c r="W339" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X339" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y339" s="0" t="s">
         <x:v>2265</x:v>
       </x:c>
@@ -30719,6 +31733,9 @@
       <x:c r="W340" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X340" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y340" s="0" t="s">
         <x:v>2265</x:v>
       </x:c>
@@ -30781,6 +31798,9 @@
       <x:c r="W341" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X341" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y341" s="0" t="s">
         <x:v>2288</x:v>
       </x:c>
@@ -30843,6 +31863,9 @@
       <x:c r="W342" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X342" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y342" s="0" t="s">
         <x:v>2288</x:v>
       </x:c>
@@ -30905,6 +31928,9 @@
       <x:c r="W343" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X343" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y343" s="0" t="s">
         <x:v>2288</x:v>
       </x:c>
@@ -30967,6 +31993,9 @@
       <x:c r="W344" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X344" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y344" s="0" t="s">
         <x:v>2288</x:v>
       </x:c>
@@ -31029,6 +32058,9 @@
       <x:c r="W345" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X345" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y345" s="0" t="s">
         <x:v>2311</x:v>
       </x:c>
@@ -31091,6 +32123,9 @@
       <x:c r="W346" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X346" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y346" s="0" t="s">
         <x:v>2319</x:v>
       </x:c>
@@ -31153,6 +32188,9 @@
       <x:c r="W347" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X347" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y347" s="0" t="s">
         <x:v>2327</x:v>
       </x:c>
@@ -31215,6 +32253,9 @@
       <x:c r="W348" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X348" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y348" s="0" t="s">
         <x:v>2327</x:v>
       </x:c>
@@ -31277,6 +32318,9 @@
       <x:c r="W349" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X349" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y349" s="0" t="s">
         <x:v>2340</x:v>
       </x:c>
@@ -31339,6 +32383,9 @@
       <x:c r="W350" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X350" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y350" s="0" t="s">
         <x:v>2340</x:v>
       </x:c>
@@ -31401,6 +32448,9 @@
       <x:c r="W351" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X351" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y351" s="0" t="s">
         <x:v>2340</x:v>
       </x:c>
@@ -31463,6 +32513,9 @@
       <x:c r="W352" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X352" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y352" s="0" t="s">
         <x:v>2340</x:v>
       </x:c>
@@ -31525,6 +32578,9 @@
       <x:c r="W353" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X353" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y353" s="0" t="s">
         <x:v>2340</x:v>
       </x:c>
@@ -31587,6 +32643,9 @@
       <x:c r="W354" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X354" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y354" s="0" t="s">
         <x:v>2368</x:v>
       </x:c>
@@ -31649,6 +32708,9 @@
       <x:c r="W355" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X355" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y355" s="0" t="s">
         <x:v>2376</x:v>
       </x:c>
@@ -31711,6 +32773,9 @@
       <x:c r="W356" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X356" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y356" s="0" t="s">
         <x:v>2376</x:v>
       </x:c>
@@ -31773,6 +32838,9 @@
       <x:c r="W357" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X357" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y357" s="0" t="s">
         <x:v>2376</x:v>
       </x:c>
@@ -31835,6 +32903,9 @@
       <x:c r="W358" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X358" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y358" s="0" t="s">
         <x:v>2376</x:v>
       </x:c>
@@ -31897,6 +32968,9 @@
       <x:c r="W359" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X359" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y359" s="0" t="s">
         <x:v>2401</x:v>
       </x:c>
@@ -31959,6 +33033,9 @@
       <x:c r="W360" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X360" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y360" s="0" t="s">
         <x:v>2401</x:v>
       </x:c>
@@ -32021,6 +33098,9 @@
       <x:c r="W361" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X361" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y361" s="0" t="s">
         <x:v>2401</x:v>
       </x:c>
@@ -32083,6 +33163,9 @@
       <x:c r="W362" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X362" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y362" s="0" t="s">
         <x:v>2401</x:v>
       </x:c>
@@ -32145,6 +33228,9 @@
       <x:c r="W363" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X363" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y363" s="0" t="s">
         <x:v>2424</x:v>
       </x:c>
@@ -32207,6 +33293,9 @@
       <x:c r="W364" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X364" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y364" s="0" t="s">
         <x:v>2424</x:v>
       </x:c>
@@ -32269,6 +33358,9 @@
       <x:c r="W365" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X365" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y365" s="0" t="s">
         <x:v>2424</x:v>
       </x:c>
@@ -32331,6 +33423,9 @@
       <x:c r="W366" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X366" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y366" s="0" t="s">
         <x:v>2424</x:v>
       </x:c>
@@ -32393,6 +33488,9 @@
       <x:c r="W367" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X367" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y367" s="0" t="s">
         <x:v>2424</x:v>
       </x:c>
@@ -32455,6 +33553,9 @@
       <x:c r="W368" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X368" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y368" s="0" t="s">
         <x:v>2451</x:v>
       </x:c>
@@ -32517,6 +33618,9 @@
       <x:c r="W369" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X369" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y369" s="0" t="s">
         <x:v>2451</x:v>
       </x:c>
@@ -32579,6 +33683,9 @@
       <x:c r="W370" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X370" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y370" s="0" t="s">
         <x:v>2451</x:v>
       </x:c>
@@ -32641,6 +33748,9 @@
       <x:c r="W371" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X371" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y371" s="0" t="s">
         <x:v>2451</x:v>
       </x:c>
@@ -32703,6 +33813,9 @@
       <x:c r="W372" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X372" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y372" s="0" t="s">
         <x:v>2451</x:v>
       </x:c>
@@ -32765,6 +33878,9 @@
       <x:c r="W373" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X373" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y373" s="0" t="s">
         <x:v>2479</x:v>
       </x:c>
@@ -32827,6 +33943,9 @@
       <x:c r="W374" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X374" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y374" s="0" t="s">
         <x:v>2487</x:v>
       </x:c>
@@ -32889,6 +34008,9 @@
       <x:c r="W375" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X375" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y375" s="0" t="s">
         <x:v>2496</x:v>
       </x:c>
@@ -32951,6 +34073,9 @@
       <x:c r="W376" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X376" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y376" s="0" t="s">
         <x:v>2496</x:v>
       </x:c>
@@ -33013,6 +34138,9 @@
       <x:c r="W377" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X377" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y377" s="0" t="s">
         <x:v>2510</x:v>
       </x:c>
@@ -33075,6 +34203,9 @@
       <x:c r="W378" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X378" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y378" s="0" t="s">
         <x:v>2510</x:v>
       </x:c>
@@ -33137,6 +34268,9 @@
       <x:c r="W379" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X379" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y379" s="0" t="s">
         <x:v>2510</x:v>
       </x:c>
@@ -33199,6 +34333,9 @@
       <x:c r="W380" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X380" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y380" s="0" t="s">
         <x:v>2510</x:v>
       </x:c>
@@ -33261,6 +34398,9 @@
       <x:c r="W381" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X381" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y381" s="0" t="s">
         <x:v>2533</x:v>
       </x:c>
@@ -33323,6 +34463,9 @@
       <x:c r="W382" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X382" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y382" s="0" t="s">
         <x:v>2533</x:v>
       </x:c>
@@ -33385,6 +34528,9 @@
       <x:c r="W383" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X383" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y383" s="0" t="s">
         <x:v>2533</x:v>
       </x:c>
@@ -33447,6 +34593,9 @@
       <x:c r="W384" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X384" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y384" s="0" t="s">
         <x:v>2533</x:v>
       </x:c>
@@ -33509,6 +34658,9 @@
       <x:c r="W385" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X385" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y385" s="0" t="s">
         <x:v>2556</x:v>
       </x:c>
@@ -33571,6 +34723,9 @@
       <x:c r="W386" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X386" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y386" s="0" t="s">
         <x:v>2564</x:v>
       </x:c>
@@ -33633,6 +34788,9 @@
       <x:c r="W387" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X387" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y387" s="0" t="s">
         <x:v>2571</x:v>
       </x:c>
@@ -33695,6 +34853,9 @@
       <x:c r="W388" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X388" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y388" s="0" t="s">
         <x:v>2581</x:v>
       </x:c>
@@ -33751,6 +34912,9 @@
       <x:c r="W389" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X389" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y389" s="0" t="s">
         <x:v>2588</x:v>
       </x:c>
@@ -33801,6 +34965,9 @@
       <x:c r="W390" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X390" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y390" s="0" t="s">
         <x:v>2593</x:v>
       </x:c>
@@ -33851,6 +35018,9 @@
       <x:c r="W391" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X391" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y391" s="0" t="s">
         <x:v>2598</x:v>
       </x:c>
@@ -33907,6 +35077,9 @@
       <x:c r="W392" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X392" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y392" s="0" t="s">
         <x:v>2604</x:v>
       </x:c>
@@ -33969,6 +35142,9 @@
       <x:c r="W393" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X393" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y393" s="0" t="s">
         <x:v>2612</x:v>
       </x:c>
@@ -34031,6 +35207,9 @@
       <x:c r="W394" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X394" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y394" s="0" t="s">
         <x:v>2619</x:v>
       </x:c>
@@ -34093,6 +35272,9 @@
       <x:c r="W395" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X395" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y395" s="0" t="s">
         <x:v>2627</x:v>
       </x:c>
@@ -34155,6 +35337,9 @@
       <x:c r="W396" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X396" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y396" s="0" t="s">
         <x:v>2635</x:v>
       </x:c>
@@ -34217,6 +35402,9 @@
       <x:c r="W397" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X397" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y397" s="0" t="s">
         <x:v>2635</x:v>
       </x:c>
@@ -34279,6 +35467,9 @@
       <x:c r="W398" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X398" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y398" s="0" t="s">
         <x:v>2648</x:v>
       </x:c>
@@ -34341,6 +35532,9 @@
       <x:c r="W399" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X399" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y399" s="0" t="s">
         <x:v>2648</x:v>
       </x:c>
@@ -34403,6 +35597,9 @@
       <x:c r="W400" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X400" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y400" s="0" t="s">
         <x:v>2661</x:v>
       </x:c>
@@ -34465,6 +35662,9 @@
       <x:c r="W401" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X401" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y401" s="0" t="s">
         <x:v>2661</x:v>
       </x:c>
@@ -34527,6 +35727,9 @@
       <x:c r="W402" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X402" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y402" s="0" t="s">
         <x:v>2661</x:v>
       </x:c>
@@ -34589,6 +35792,9 @@
       <x:c r="W403" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X403" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y403" s="0" t="s">
         <x:v>2680</x:v>
       </x:c>
@@ -34651,6 +35857,9 @@
       <x:c r="W404" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X404" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y404" s="0" t="s">
         <x:v>2680</x:v>
       </x:c>
@@ -34713,6 +35922,9 @@
       <x:c r="W405" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X405" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y405" s="0" t="s">
         <x:v>2680</x:v>
       </x:c>
@@ -34775,6 +35987,9 @@
       <x:c r="W406" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X406" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y406" s="0" t="s">
         <x:v>2680</x:v>
       </x:c>
@@ -34837,6 +36052,9 @@
       <x:c r="W407" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X407" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y407" s="0" t="s">
         <x:v>2705</x:v>
       </x:c>
@@ -34899,6 +36117,9 @@
       <x:c r="W408" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X408" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y408" s="0" t="s">
         <x:v>2705</x:v>
       </x:c>
@@ -34961,6 +36182,9 @@
       <x:c r="W409" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X409" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y409" s="0" t="s">
         <x:v>2705</x:v>
       </x:c>
@@ -35023,6 +36247,9 @@
       <x:c r="W410" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X410" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y410" s="0" t="s">
         <x:v>2723</x:v>
       </x:c>
@@ -35085,6 +36312,9 @@
       <x:c r="W411" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X411" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y411" s="0" t="s">
         <x:v>2723</x:v>
       </x:c>
@@ -35147,6 +36377,9 @@
       <x:c r="W412" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X412" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y412" s="0" t="s">
         <x:v>2723</x:v>
       </x:c>
@@ -35209,6 +36442,9 @@
       <x:c r="W413" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X413" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y413" s="0" t="s">
         <x:v>2741</x:v>
       </x:c>
@@ -35271,6 +36507,9 @@
       <x:c r="W414" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X414" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y414" s="0" t="s">
         <x:v>2741</x:v>
       </x:c>
@@ -35333,6 +36572,9 @@
       <x:c r="W415" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X415" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y415" s="0" t="s">
         <x:v>2741</x:v>
       </x:c>
@@ -35395,6 +36637,9 @@
       <x:c r="W416" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X416" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y416" s="0" t="s">
         <x:v>2758</x:v>
       </x:c>
@@ -35457,6 +36702,9 @@
       <x:c r="W417" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X417" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y417" s="0" t="s">
         <x:v>2758</x:v>
       </x:c>
@@ -35519,6 +36767,9 @@
       <x:c r="W418" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X418" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y418" s="0" t="s">
         <x:v>2758</x:v>
       </x:c>
@@ -35581,6 +36832,9 @@
       <x:c r="W419" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X419" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y419" s="0" t="s">
         <x:v>2777</x:v>
       </x:c>
@@ -35643,6 +36897,9 @@
       <x:c r="W420" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X420" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y420" s="0" t="s">
         <x:v>2777</x:v>
       </x:c>
@@ -35705,6 +36962,9 @@
       <x:c r="W421" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X421" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y421" s="0" t="s">
         <x:v>2777</x:v>
       </x:c>
@@ -35767,6 +37027,9 @@
       <x:c r="W422" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X422" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y422" s="0" t="s">
         <x:v>2797</x:v>
       </x:c>
@@ -35829,6 +37092,9 @@
       <x:c r="W423" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X423" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y423" s="0" t="s">
         <x:v>2797</x:v>
       </x:c>
@@ -35891,6 +37157,9 @@
       <x:c r="W424" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X424" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y424" s="0" t="s">
         <x:v>2797</x:v>
       </x:c>
@@ -35953,6 +37222,9 @@
       <x:c r="W425" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X425" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y425" s="0" t="s">
         <x:v>2797</x:v>
       </x:c>
@@ -36015,6 +37287,9 @@
       <x:c r="W426" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X426" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y426" s="0" t="s">
         <x:v>2822</x:v>
       </x:c>
@@ -36077,6 +37352,9 @@
       <x:c r="W427" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X427" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y427" s="0" t="s">
         <x:v>2830</x:v>
       </x:c>
@@ -36139,6 +37417,9 @@
       <x:c r="W428" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X428" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y428" s="0" t="s">
         <x:v>2838</x:v>
       </x:c>
@@ -36201,6 +37482,9 @@
       <x:c r="W429" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X429" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y429" s="0" t="s">
         <x:v>2846</x:v>
       </x:c>
@@ -36263,6 +37547,9 @@
       <x:c r="W430" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X430" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y430" s="0" t="s">
         <x:v>2855</x:v>
       </x:c>
@@ -36325,6 +37612,9 @@
       <x:c r="W431" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X431" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y431" s="0" t="s">
         <x:v>2864</x:v>
       </x:c>
@@ -36387,6 +37677,9 @@
       <x:c r="W432" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X432" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y432" s="0" t="s">
         <x:v>2874</x:v>
       </x:c>
@@ -36449,6 +37742,9 @@
       <x:c r="W433" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X433" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y433" s="0" t="s">
         <x:v>2874</x:v>
       </x:c>
@@ -36511,6 +37807,9 @@
       <x:c r="W434" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X434" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y434" s="0" t="s">
         <x:v>2874</x:v>
       </x:c>
@@ -36573,6 +37872,9 @@
       <x:c r="W435" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X435" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y435" s="0" t="s">
         <x:v>2892</x:v>
       </x:c>
@@ -36635,6 +37937,9 @@
       <x:c r="W436" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X436" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y436" s="0" t="s">
         <x:v>2901</x:v>
       </x:c>
@@ -36697,6 +38002,9 @@
       <x:c r="W437" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X437" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y437" s="0" t="s">
         <x:v>2901</x:v>
       </x:c>
@@ -36759,6 +38067,9 @@
       <x:c r="W438" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X438" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y438" s="0" t="s">
         <x:v>2901</x:v>
       </x:c>
@@ -36821,6 +38132,9 @@
       <x:c r="W439" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X439" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y439" s="0" t="s">
         <x:v>2920</x:v>
       </x:c>
@@ -36883,6 +38197,9 @@
       <x:c r="W440" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X440" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y440" s="0" t="s">
         <x:v>2920</x:v>
       </x:c>
@@ -36945,6 +38262,9 @@
       <x:c r="W441" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X441" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y441" s="0" t="s">
         <x:v>2920</x:v>
       </x:c>
@@ -37007,6 +38327,9 @@
       <x:c r="W442" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X442" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y442" s="0" t="s">
         <x:v>2938</x:v>
       </x:c>
@@ -37069,6 +38392,9 @@
       <x:c r="W443" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X443" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y443" s="0" t="s">
         <x:v>2938</x:v>
       </x:c>
@@ -37131,6 +38457,9 @@
       <x:c r="W444" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X444" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y444" s="0" t="s">
         <x:v>2938</x:v>
       </x:c>
@@ -37193,6 +38522,9 @@
       <x:c r="W445" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X445" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y445" s="0" t="s">
         <x:v>2957</x:v>
       </x:c>
@@ -37255,6 +38587,9 @@
       <x:c r="W446" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X446" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y446" s="0" t="s">
         <x:v>2957</x:v>
       </x:c>
@@ -37317,6 +38652,9 @@
       <x:c r="W447" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X447" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y447" s="0" t="s">
         <x:v>2957</x:v>
       </x:c>
@@ -37379,6 +38717,9 @@
       <x:c r="W448" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X448" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y448" s="0" t="s">
         <x:v>2974</x:v>
       </x:c>
@@ -37441,6 +38782,9 @@
       <x:c r="W449" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X449" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y449" s="0" t="s">
         <x:v>2982</x:v>
       </x:c>
@@ -37503,6 +38847,9 @@
       <x:c r="W450" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X450" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y450" s="0" t="s">
         <x:v>2982</x:v>
       </x:c>
@@ -37565,6 +38912,9 @@
       <x:c r="W451" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X451" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y451" s="0" t="s">
         <x:v>2982</x:v>
       </x:c>
@@ -37627,6 +38977,9 @@
       <x:c r="W452" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X452" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y452" s="0" t="s">
         <x:v>2982</x:v>
       </x:c>
@@ -37689,6 +39042,9 @@
       <x:c r="W453" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X453" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y453" s="0" t="s">
         <x:v>3009</x:v>
       </x:c>
@@ -37751,6 +39107,9 @@
       <x:c r="W454" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X454" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y454" s="0" t="s">
         <x:v>3009</x:v>
       </x:c>
@@ -37813,6 +39172,9 @@
       <x:c r="W455" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X455" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y455" s="0" t="s">
         <x:v>3009</x:v>
       </x:c>
@@ -37875,6 +39237,9 @@
       <x:c r="W456" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X456" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y456" s="0" t="s">
         <x:v>3009</x:v>
       </x:c>
@@ -37937,6 +39302,9 @@
       <x:c r="W457" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X457" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y457" s="0" t="s">
         <x:v>3009</x:v>
       </x:c>
@@ -37999,6 +39367,9 @@
       <x:c r="W458" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X458" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y458" s="0" t="s">
         <x:v>3041</x:v>
       </x:c>
@@ -38061,6 +39432,9 @@
       <x:c r="W459" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X459" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y459" s="0" t="s">
         <x:v>3041</x:v>
       </x:c>
@@ -38123,6 +39497,9 @@
       <x:c r="W460" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X460" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y460" s="0" t="s">
         <x:v>3041</x:v>
       </x:c>
@@ -38185,6 +39562,9 @@
       <x:c r="W461" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X461" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y461" s="0" t="s">
         <x:v>3041</x:v>
       </x:c>
@@ -38247,6 +39627,9 @@
       <x:c r="W462" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X462" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y462" s="0" t="s">
         <x:v>3041</x:v>
       </x:c>
@@ -38309,6 +39692,9 @@
       <x:c r="W463" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X463" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y463" s="0" t="s">
         <x:v>3073</x:v>
       </x:c>
@@ -38371,6 +39757,9 @@
       <x:c r="W464" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X464" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y464" s="0" t="s">
         <x:v>3073</x:v>
       </x:c>
@@ -38433,6 +39822,9 @@
       <x:c r="W465" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X465" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y465" s="0" t="s">
         <x:v>3073</x:v>
       </x:c>
@@ -38495,6 +39887,9 @@
       <x:c r="W466" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X466" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y466" s="0" t="s">
         <x:v>3073</x:v>
       </x:c>
@@ -38557,6 +39952,9 @@
       <x:c r="W467" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X467" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y467" s="0" t="s">
         <x:v>3097</x:v>
       </x:c>
@@ -38619,6 +40017,9 @@
       <x:c r="W468" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X468" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y468" s="0" t="s">
         <x:v>3097</x:v>
       </x:c>
@@ -38681,6 +40082,9 @@
       <x:c r="W469" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X469" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y469" s="0" t="s">
         <x:v>3097</x:v>
       </x:c>
@@ -38743,6 +40147,9 @@
       <x:c r="W470" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X470" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y470" s="0" t="s">
         <x:v>3097</x:v>
       </x:c>
@@ -38805,6 +40212,9 @@
       <x:c r="W471" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X471" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y471" s="0" t="s">
         <x:v>3120</x:v>
       </x:c>
@@ -38867,6 +40277,9 @@
       <x:c r="W472" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X472" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y472" s="0" t="s">
         <x:v>3120</x:v>
       </x:c>
@@ -38929,6 +40342,9 @@
       <x:c r="W473" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X473" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y473" s="0" t="s">
         <x:v>3120</x:v>
       </x:c>
@@ -38991,6 +40407,9 @@
       <x:c r="W474" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X474" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y474" s="0" t="s">
         <x:v>3138</x:v>
       </x:c>
@@ -39053,6 +40472,9 @@
       <x:c r="W475" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X475" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y475" s="0" t="s">
         <x:v>3138</x:v>
       </x:c>
@@ -39115,6 +40537,9 @@
       <x:c r="W476" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X476" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y476" s="0" t="s">
         <x:v>3138</x:v>
       </x:c>
@@ -39177,6 +40602,9 @@
       <x:c r="W477" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X477" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y477" s="0" t="s">
         <x:v>3156</x:v>
       </x:c>
@@ -39239,6 +40667,9 @@
       <x:c r="W478" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X478" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y478" s="0" t="s">
         <x:v>3156</x:v>
       </x:c>
@@ -39301,6 +40732,9 @@
       <x:c r="W479" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X479" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y479" s="0" t="s">
         <x:v>3156</x:v>
       </x:c>
@@ -39363,6 +40797,9 @@
       <x:c r="W480" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X480" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y480" s="0" t="s">
         <x:v>3173</x:v>
       </x:c>
@@ -39425,6 +40862,9 @@
       <x:c r="W481" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X481" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y481" s="0" t="s">
         <x:v>3173</x:v>
       </x:c>
@@ -39487,6 +40927,9 @@
       <x:c r="W482" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X482" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y482" s="0" t="s">
         <x:v>3173</x:v>
       </x:c>
@@ -39549,6 +40992,9 @@
       <x:c r="W483" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X483" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y483" s="0" t="s">
         <x:v>3190</x:v>
       </x:c>
@@ -39611,6 +41057,9 @@
       <x:c r="W484" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="X484" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="Y484" s="0" t="s">
         <x:v>3199</x:v>
       </x:c>
@@ -39666,6 +41115,9 @@
       </x:c>
       <x:c r="W485" s="0" t="n">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="X485" s="0" t="n">
+        <x:v>14</x:v>
       </x:c>
       <x:c r="Y485" s="0" t="s">
         <x:v>3207</x:v>

</xml_diff>